<commit_message>
Ngọc coi lại ik
</commit_message>
<xml_diff>
--- a/Bản kế hoạch.xlsx
+++ b/Bản kế hoạch.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dowload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\cay-nhi-phan\cay-nhi-phan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F09871-2EF3-48F6-B2D6-3052EDB7808D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61C8268-7B5E-4F51-AF76-ACD9304DEC35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
   <si>
     <t>STT</t>
   </si>
@@ -122,48 +122,6 @@
   </si>
   <si>
     <t>30/10/2018</t>
-  </si>
-  <si>
-    <t>19/9/2019</t>
-  </si>
-  <si>
-    <t>19/9/2020</t>
-  </si>
-  <si>
-    <t>19/9/2021</t>
-  </si>
-  <si>
-    <t>19/9/2022</t>
-  </si>
-  <si>
-    <t>19/9/2023</t>
-  </si>
-  <si>
-    <t>19/9/2024</t>
-  </si>
-  <si>
-    <t>19/9/2025</t>
-  </si>
-  <si>
-    <t>30/9/2019</t>
-  </si>
-  <si>
-    <t>30/9/2020</t>
-  </si>
-  <si>
-    <t>30/9/2021</t>
-  </si>
-  <si>
-    <t>30/9/2022</t>
-  </si>
-  <si>
-    <t>30/9/2023</t>
-  </si>
-  <si>
-    <t>30/9/2024</t>
-  </si>
-  <si>
-    <t>30/9/2025</t>
   </si>
   <si>
     <t>27/9/2018</t>
@@ -365,6 +323,9 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -394,9 +355,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,8 +641,8 @@
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -700,24 +658,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
@@ -741,10 +699,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" s="8" customFormat="1">
-      <c r="A3" s="26">
+      <c r="A3" s="27">
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="28" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -769,8 +727,8 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" s="8" customFormat="1">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
@@ -782,19 +740,19 @@
         <v>43291</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" s="8" customFormat="1">
-      <c r="A5" s="26"/>
-      <c r="B5" s="27"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
@@ -806,19 +764,19 @@
         <v>43292</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" s="8" customFormat="1">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
@@ -830,19 +788,19 @@
         <v>43293</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" s="8" customFormat="1">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="5" t="s">
         <v>23</v>
       </c>
@@ -856,19 +814,19 @@
         <v>43294</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" s="8" customFormat="1">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="13" t="s">
         <v>15</v>
       </c>
@@ -882,19 +840,19 @@
         <v>43295</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" s="8" customFormat="1">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
@@ -908,19 +866,19 @@
         <v>43296</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" s="8" customFormat="1">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="5" t="s">
         <v>16</v>
       </c>
@@ -934,21 +892,21 @@
         <v>43297</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" s="12" customFormat="1">
-      <c r="A11" s="20">
+      <c r="A11" s="21">
         <v>2</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="23" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -973,8 +931,8 @@
       <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" s="12" customFormat="1">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="9" t="s">
         <v>26</v>
       </c>
@@ -990,15 +948,15 @@
       <c r="G12" s="18">
         <v>43291</v>
       </c>
-      <c r="H12" s="30" t="s">
-        <v>49</v>
+      <c r="H12" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:10" s="12" customFormat="1">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="9" t="s">
         <v>25</v>
       </c>
@@ -1012,15 +970,15 @@
       <c r="G13" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="30" t="s">
-        <v>48</v>
+      <c r="H13" s="20" t="s">
+        <v>34</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
     </row>
     <row r="14" spans="1:10" s="12" customFormat="1">
-      <c r="A14" s="21"/>
-      <c r="B14" s="23"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="9" t="s">
         <v>10</v>
       </c>
@@ -1034,17 +992,17 @@
       <c r="G14" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="30" t="s">
-        <v>48</v>
+      <c r="H14" s="20" t="s">
+        <v>34</v>
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
     </row>
     <row r="15" spans="1:10" s="17" customFormat="1">
-      <c r="A15" s="20">
+      <c r="A15" s="21">
         <v>3</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="23" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="14" t="s">
@@ -1065,8 +1023,8 @@
       <c r="J15" s="16"/>
     </row>
     <row r="16" spans="1:10" s="17" customFormat="1">
-      <c r="A16" s="21"/>
-      <c r="B16" s="23"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="14" t="s">
         <v>32</v>
       </c>

</xml_diff>